<commit_message>
Banyak banget Same luna
</commit_message>
<xml_diff>
--- a/assets/upload/Program.xlsx
+++ b/assets/upload/Program.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1274" uniqueCount="462">
   <si>
     <t>SUBINITIATIVE_NAME</t>
   </si>
@@ -1272,33 +1272,6 @@
     <t>INITIATIVE_NO</t>
   </si>
   <si>
-    <t>1a.</t>
-  </si>
-  <si>
-    <t>1b.</t>
-  </si>
-  <si>
-    <t>1c.</t>
-  </si>
-  <si>
-    <t>1d.</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>2.2</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t>6a.</t>
-  </si>
-  <si>
     <t>6b.1</t>
   </si>
   <si>
@@ -1308,36 +1281,12 @@
     <t>6c</t>
   </si>
   <si>
-    <t>7a.</t>
-  </si>
-  <si>
-    <t>7b.</t>
-  </si>
-  <si>
-    <t>7c.</t>
-  </si>
-  <si>
     <t>14a</t>
   </si>
   <si>
     <t>14b</t>
   </si>
   <si>
-    <t>17a.</t>
-  </si>
-  <si>
-    <t>17b.</t>
-  </si>
-  <si>
-    <t>19a.</t>
-  </si>
-  <si>
-    <t>19b.</t>
-  </si>
-  <si>
-    <t>19c.</t>
-  </si>
-  <si>
     <t>Deepen client relationship</t>
   </si>
   <si>
@@ -1375,6 +1324,108 @@
   </si>
   <si>
     <t>Ogi Prastomiyono</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>1c</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>6a</t>
+  </si>
+  <si>
+    <t>7a</t>
+  </si>
+  <si>
+    <t>7b</t>
+  </si>
+  <si>
+    <t>7c</t>
+  </si>
+  <si>
+    <t>17a</t>
+  </si>
+  <si>
+    <t>17b</t>
+  </si>
+  <si>
+    <t>19a</t>
+  </si>
+  <si>
+    <t>19b</t>
+  </si>
+  <si>
+    <t>19c</t>
+  </si>
+  <si>
+    <t>PMO Head</t>
+  </si>
+  <si>
+    <t>Rustam S.  Sirait</t>
+  </si>
+  <si>
+    <t>Myland</t>
+  </si>
+  <si>
+    <t>Angga Erlangga  Hanafie</t>
+  </si>
+  <si>
+    <t>Harry Gale</t>
+  </si>
+  <si>
+    <t>Wawan Setiawan</t>
+  </si>
+  <si>
+    <t>Anton Herdianto</t>
+  </si>
+  <si>
+    <t>Iswahyudi</t>
+  </si>
+  <si>
+    <t>Farida Thamrin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n/a </t>
+  </si>
+  <si>
+    <t>Pantro Pader Silitonga</t>
+  </si>
+  <si>
+    <t>Elina Wirjakusuma</t>
+  </si>
+  <si>
+    <t>Tedi Nurhikmat</t>
+  </si>
+  <si>
+    <t>Rustam S Sirait</t>
+  </si>
+  <si>
+    <t>Rahmat Broto Triaji</t>
+  </si>
+  <si>
+    <t>Adinata Widia</t>
+  </si>
+  <si>
+    <t>Mohammad Guntur</t>
+  </si>
+  <si>
+    <t>Anita Widjaja</t>
+  </si>
+  <si>
+    <t>Elmamber Petamu Sinaga</t>
+  </si>
+  <si>
+    <t>Rohan Hafas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wawan Setiawan </t>
   </si>
 </sst>
 </file>
@@ -1418,7 +1469,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1441,11 +1492,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1472,6 +1551,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1751,10 +1839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F195"/>
+  <dimension ref="A1:G195"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1771,7 +1859,7 @@
     <col min="10" max="10" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>405</v>
       </c>
@@ -1788,12 +1876,15 @@
         <v>409</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>418</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>372</v>
@@ -1805,15 +1896,18 @@
         <v>178</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>372</v>
@@ -1825,15 +1919,18 @@
         <v>179</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>372</v>
@@ -1845,15 +1942,18 @@
         <v>180</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>372</v>
@@ -1865,15 +1965,18 @@
         <v>181</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>372</v>
@@ -1885,15 +1988,18 @@
         <v>182</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>372</v>
@@ -1905,15 +2011,18 @@
         <v>183</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>373</v>
@@ -1925,15 +2034,18 @@
         <v>184</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>373</v>
@@ -1945,15 +2057,18 @@
         <v>185</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>373</v>
@@ -1965,15 +2080,18 @@
         <v>186</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>373</v>
@@ -1985,15 +2103,18 @@
         <v>187</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>374</v>
@@ -2005,15 +2126,18 @@
         <v>188</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>412</v>
+        <v>430</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>374</v>
@@ -2025,15 +2149,18 @@
         <v>189</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>412</v>
+        <v>430</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>374</v>
@@ -2045,15 +2172,18 @@
         <v>190</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>412</v>
+        <v>430</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>374</v>
@@ -2065,15 +2195,18 @@
         <v>191</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>412</v>
+        <v>430</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>375</v>
@@ -2085,15 +2218,18 @@
         <v>192</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>375</v>
@@ -2105,15 +2241,18 @@
         <v>193</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>375</v>
@@ -2125,15 +2264,18 @@
         <v>194</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>375</v>
@@ -2145,15 +2287,18 @@
         <v>195</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>375</v>
@@ -2165,15 +2310,18 @@
         <v>196</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>375</v>
@@ -2185,15 +2333,18 @@
         <v>197</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>375</v>
@@ -2205,15 +2356,18 @@
         <v>198</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+        <v>417</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>376</v>
@@ -2224,16 +2378,19 @@
       <c r="D23" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>414</v>
+      <c r="E23" s="6">
+        <v>2.1</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>376</v>
@@ -2244,16 +2401,19 @@
       <c r="D24" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="E24" s="6" t="s">
-        <v>414</v>
+      <c r="E24" s="6">
+        <v>2.1</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G24" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>376</v>
@@ -2264,16 +2424,19 @@
       <c r="D25" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="E25" s="6" t="s">
-        <v>414</v>
+      <c r="E25" s="6">
+        <v>2.1</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>376</v>
@@ -2284,16 +2447,19 @@
       <c r="D26" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E26" s="6" t="s">
-        <v>414</v>
+      <c r="E26" s="6">
+        <v>2.1</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>376</v>
@@ -2304,16 +2470,19 @@
       <c r="D27" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>414</v>
+      <c r="E27" s="6">
+        <v>2.1</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>377</v>
@@ -2324,16 +2493,19 @@
       <c r="D28" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>415</v>
+      <c r="E28" s="6">
+        <v>2.2000000000000002</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>377</v>
@@ -2344,16 +2516,19 @@
       <c r="D29" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>415</v>
+      <c r="E29" s="6">
+        <v>2.2000000000000002</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>377</v>
@@ -2364,16 +2539,19 @@
       <c r="D30" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>415</v>
+      <c r="E30" s="6">
+        <v>2.2000000000000002</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>378</v>
@@ -2384,16 +2562,19 @@
       <c r="D31" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="E31" s="6">
+        <v>3</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="G31" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>378</v>
@@ -2404,16 +2585,19 @@
       <c r="D32" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="6">
+        <v>3</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="G32" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>378</v>
@@ -2424,16 +2608,19 @@
       <c r="D33" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" s="6">
+        <v>3</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="G33" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>378</v>
@@ -2444,16 +2631,19 @@
       <c r="D34" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="6">
+        <v>3</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="G34" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="F34" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>378</v>
@@ -2464,16 +2654,19 @@
       <c r="D35" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="E35" s="6" t="s">
+      <c r="E35" s="6">
+        <v>3</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="G35" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>378</v>
@@ -2484,16 +2677,19 @@
       <c r="D36" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E36" s="6" t="s">
+      <c r="E36" s="6">
+        <v>3</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>416</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>433</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>379</v>
@@ -2508,12 +2704,15 @@
         <v>4</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>379</v>
@@ -2528,12 +2727,15 @@
         <v>4</v>
       </c>
       <c r="F38" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>379</v>
@@ -2548,12 +2750,15 @@
         <v>4</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>379</v>
@@ -2568,12 +2773,15 @@
         <v>4</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>379</v>
@@ -2588,12 +2796,15 @@
         <v>4</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>379</v>
@@ -2608,12 +2819,15 @@
         <v>4</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G42" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>380</v>
@@ -2624,16 +2838,19 @@
       <c r="D43" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="E43" s="6" t="s">
-        <v>417</v>
+      <c r="E43" s="6">
+        <v>5</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>380</v>
@@ -2644,16 +2861,19 @@
       <c r="D44" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="E44" s="6" t="s">
-        <v>417</v>
+      <c r="E44" s="6">
+        <v>5</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>380</v>
@@ -2664,16 +2884,19 @@
       <c r="D45" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="E45" s="6" t="s">
-        <v>417</v>
+      <c r="E45" s="6">
+        <v>5</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>380</v>
@@ -2684,16 +2907,19 @@
       <c r="D46" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>417</v>
+      <c r="E46" s="6">
+        <v>5</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>380</v>
@@ -2704,16 +2930,19 @@
       <c r="D47" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="E47" s="6" t="s">
-        <v>417</v>
+      <c r="E47" s="6">
+        <v>5</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G47" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>380</v>
@@ -2724,16 +2953,19 @@
       <c r="D48" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="E48" s="6" t="s">
-        <v>417</v>
+      <c r="E48" s="6">
+        <v>5</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>380</v>
@@ -2744,16 +2976,19 @@
       <c r="D49" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="E49" s="6" t="s">
-        <v>417</v>
+      <c r="E49" s="6">
+        <v>5</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>380</v>
@@ -2764,16 +2999,19 @@
       <c r="D50" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="E50" s="6" t="s">
-        <v>417</v>
+      <c r="E50" s="6">
+        <v>5</v>
       </c>
       <c r="F50" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>433</v>
+        <v>416</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>380</v>
@@ -2784,16 +3022,19 @@
       <c r="D51" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E51" s="6" t="s">
-        <v>417</v>
+      <c r="E51" s="6">
+        <v>5</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G51" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>381</v>
@@ -2805,15 +3046,18 @@
         <v>228</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="F52" s="9" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+      <c r="G52" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>381</v>
@@ -2825,15 +3069,18 @@
         <v>229</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+      <c r="G53" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>381</v>
@@ -2845,15 +3092,18 @@
         <v>230</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+      <c r="G54" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>381</v>
@@ -2865,15 +3115,18 @@
         <v>231</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>381</v>
@@ -2885,15 +3138,18 @@
         <v>232</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>418</v>
+        <v>432</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>420</v>
+      </c>
+      <c r="G56" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>382</v>
@@ -2905,15 +3161,18 @@
         <v>233</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>382</v>
@@ -2925,15 +3184,18 @@
         <v>234</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="F58" s="9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G58" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>382</v>
@@ -2945,15 +3207,18 @@
         <v>235</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G59" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>382</v>
@@ -2965,15 +3230,18 @@
         <v>236</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G60" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>382</v>
@@ -2985,15 +3253,18 @@
         <v>237</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G61" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>383</v>
@@ -3005,15 +3276,18 @@
         <v>238</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="F62" s="9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G62" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>383</v>
@@ -3025,15 +3299,18 @@
         <v>239</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G63" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>383</v>
@@ -3045,15 +3322,18 @@
         <v>240</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>383</v>
@@ -3065,15 +3345,18 @@
         <v>241</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G65" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>383</v>
@@ -3085,15 +3368,18 @@
         <v>242</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+      <c r="G66" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>384</v>
@@ -3105,15 +3391,18 @@
         <v>243</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F67" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G67" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>384</v>
@@ -3125,15 +3414,18 @@
         <v>244</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F68" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G68" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>384</v>
@@ -3145,15 +3437,18 @@
         <v>245</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G69" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>384</v>
@@ -3165,15 +3460,18 @@
         <v>246</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G70" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>384</v>
@@ -3185,15 +3483,18 @@
         <v>247</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G71" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>384</v>
@@ -3205,15 +3506,18 @@
         <v>248</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F72" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G72" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>384</v>
@@ -3225,15 +3529,18 @@
         <v>249</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F73" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G73" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>384</v>
@@ -3245,15 +3552,18 @@
         <v>250</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F74" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G74" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>384</v>
@@ -3265,15 +3575,18 @@
         <v>251</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G75" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>432</v>
+        <v>415</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>384</v>
@@ -3285,13 +3598,16 @@
         <v>252</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G76" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>406</v>
       </c>
@@ -3305,13 +3621,16 @@
         <v>253</v>
       </c>
       <c r="E77" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="F77" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="F77" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G77" s="11" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>406</v>
       </c>
@@ -3325,13 +3644,16 @@
         <v>254</v>
       </c>
       <c r="E78" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="F78" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="F78" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G78" s="11" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>406</v>
       </c>
@@ -3345,13 +3667,16 @@
         <v>255</v>
       </c>
       <c r="E79" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="F79" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="F79" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G79" s="11" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>406</v>
       </c>
@@ -3365,13 +3690,16 @@
         <v>256</v>
       </c>
       <c r="E80" s="6" t="s">
+        <v>433</v>
+      </c>
+      <c r="F80" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="F80" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G80" s="11" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>406</v>
       </c>
@@ -3385,13 +3713,16 @@
         <v>257</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="F81" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G81" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>406</v>
       </c>
@@ -3405,13 +3736,16 @@
         <v>258</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="F82" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G82" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>406</v>
       </c>
@@ -3425,13 +3759,16 @@
         <v>259</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G83" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>406</v>
       </c>
@@ -3445,13 +3782,16 @@
         <v>260</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>406</v>
       </c>
@@ -3465,13 +3805,16 @@
         <v>261</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>406</v>
       </c>
@@ -3485,13 +3828,16 @@
         <v>262</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="F86" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G86" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>406</v>
       </c>
@@ -3505,13 +3851,16 @@
         <v>263</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G87" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>406</v>
       </c>
@@ -3525,13 +3874,16 @@
         <v>264</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>423</v>
+        <v>434</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G88" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>406</v>
       </c>
@@ -3545,13 +3897,16 @@
         <v>265</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G89" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>406</v>
       </c>
@@ -3565,13 +3920,16 @@
         <v>266</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G90" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>406</v>
       </c>
@@ -3585,13 +3943,16 @@
         <v>267</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G91" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>406</v>
       </c>
@@ -3605,13 +3966,16 @@
         <v>268</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>406</v>
       </c>
@@ -3625,13 +3989,16 @@
         <v>269</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G93" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>406</v>
       </c>
@@ -3645,13 +4012,16 @@
         <v>270</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G94" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>406</v>
       </c>
@@ -3665,13 +4035,16 @@
         <v>271</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>424</v>
+        <v>435</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G95" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>406</v>
       </c>
@@ -3688,10 +4061,13 @@
         <v>8</v>
       </c>
       <c r="F96" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G96" s="11" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>406</v>
       </c>
@@ -3708,10 +4084,13 @@
         <v>8</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G97" s="11" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>406</v>
       </c>
@@ -3728,10 +4107,13 @@
         <v>8</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G98" s="11" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>407</v>
       </c>
@@ -3748,10 +4130,13 @@
         <v>9</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G99" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>407</v>
       </c>
@@ -3768,10 +4153,13 @@
         <v>9</v>
       </c>
       <c r="F100" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G100" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>407</v>
       </c>
@@ -3788,10 +4176,13 @@
         <v>9</v>
       </c>
       <c r="F101" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G101" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>407</v>
       </c>
@@ -3808,10 +4199,13 @@
         <v>9</v>
       </c>
       <c r="F102" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G102" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>407</v>
       </c>
@@ -3828,10 +4222,13 @@
         <v>9</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G103" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>407</v>
       </c>
@@ -3848,10 +4245,13 @@
         <v>9</v>
       </c>
       <c r="F104" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G104" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>407</v>
       </c>
@@ -3868,10 +4268,13 @@
         <v>9</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G105" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>407</v>
       </c>
@@ -3888,10 +4291,13 @@
         <v>9</v>
       </c>
       <c r="F106" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G106" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>407</v>
       </c>
@@ -3908,10 +4314,13 @@
         <v>9</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G107" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>407</v>
       </c>
@@ -3928,10 +4337,13 @@
         <v>9</v>
       </c>
       <c r="F108" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G108" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>407</v>
       </c>
@@ -3948,10 +4360,13 @@
         <v>9</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>423</v>
+      </c>
+      <c r="G109" s="12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>407</v>
       </c>
@@ -3968,10 +4383,13 @@
         <v>10</v>
       </c>
       <c r="F110" s="9" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+      <c r="G110" s="12" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="2" t="s">
         <v>407</v>
       </c>
@@ -3988,10 +4406,13 @@
         <v>10</v>
       </c>
       <c r="F111" s="9" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+      <c r="G111" s="12" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A112" s="2" t="s">
         <v>407</v>
       </c>
@@ -4008,10 +4429,13 @@
         <v>11</v>
       </c>
       <c r="F112" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A113" s="2" t="s">
         <v>407</v>
       </c>
@@ -4028,10 +4452,13 @@
         <v>11</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G113" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A114" s="2" t="s">
         <v>407</v>
       </c>
@@ -4048,10 +4475,13 @@
         <v>11</v>
       </c>
       <c r="F114" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G114" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="2" t="s">
         <v>407</v>
       </c>
@@ -4068,10 +4498,13 @@
         <v>12</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G115" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A116" s="2" t="s">
         <v>407</v>
       </c>
@@ -4088,10 +4521,13 @@
         <v>12</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G116" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
         <v>407</v>
       </c>
@@ -4108,10 +4544,13 @@
         <v>12</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G117" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
         <v>407</v>
       </c>
@@ -4128,10 +4567,13 @@
         <v>12</v>
       </c>
       <c r="F118" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
         <v>407</v>
       </c>
@@ -4148,10 +4590,13 @@
         <v>12</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G119" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
         <v>407</v>
       </c>
@@ -4168,10 +4613,13 @@
         <v>12</v>
       </c>
       <c r="F120" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G120" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
         <v>407</v>
       </c>
@@ -4188,10 +4636,13 @@
         <v>12</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
         <v>407</v>
       </c>
@@ -4208,10 +4659,13 @@
         <v>12</v>
       </c>
       <c r="F122" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G122" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
         <v>407</v>
       </c>
@@ -4228,10 +4682,13 @@
         <v>12</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G123" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
         <v>407</v>
       </c>
@@ -4248,10 +4705,13 @@
         <v>12</v>
       </c>
       <c r="F124" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G124" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
         <v>407</v>
       </c>
@@ -4268,10 +4728,13 @@
         <v>12</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G125" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
         <v>407</v>
       </c>
@@ -4288,10 +4751,13 @@
         <v>12</v>
       </c>
       <c r="F126" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G126" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
         <v>407</v>
       </c>
@@ -4308,10 +4774,13 @@
         <v>12</v>
       </c>
       <c r="F127" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G127" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
         <v>407</v>
       </c>
@@ -4328,10 +4797,13 @@
         <v>12</v>
       </c>
       <c r="F128" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G128" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
         <v>407</v>
       </c>
@@ -4348,10 +4820,13 @@
         <v>12</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G129" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
         <v>407</v>
       </c>
@@ -4368,10 +4843,13 @@
         <v>12</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G130" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A131" s="2" t="s">
         <v>407</v>
       </c>
@@ -4388,10 +4866,13 @@
         <v>12</v>
       </c>
       <c r="F131" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G131" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
         <v>407</v>
       </c>
@@ -4408,10 +4889,13 @@
         <v>12</v>
       </c>
       <c r="F132" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G132" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
         <v>407</v>
       </c>
@@ -4428,10 +4912,13 @@
         <v>12</v>
       </c>
       <c r="F133" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G133" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
         <v>407</v>
       </c>
@@ -4448,10 +4935,13 @@
         <v>12</v>
       </c>
       <c r="F134" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G134" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>407</v>
       </c>
@@ -4468,10 +4958,13 @@
         <v>12</v>
       </c>
       <c r="F135" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G135" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
         <v>407</v>
       </c>
@@ -4488,10 +4981,13 @@
         <v>12</v>
       </c>
       <c r="F136" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G136" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
         <v>407</v>
       </c>
@@ -4508,10 +5004,13 @@
         <v>12</v>
       </c>
       <c r="F137" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G137" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
         <v>407</v>
       </c>
@@ -4528,10 +5027,13 @@
         <v>13</v>
       </c>
       <c r="F138" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G138" s="11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A139" s="2" t="s">
         <v>407</v>
       </c>
@@ -4548,10 +5050,13 @@
         <v>13</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G139" s="11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
         <v>407</v>
       </c>
@@ -4568,10 +5073,13 @@
         <v>13</v>
       </c>
       <c r="F140" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G140" s="11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>407</v>
       </c>
@@ -4588,10 +5096,13 @@
         <v>13</v>
       </c>
       <c r="F141" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G141" s="11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
         <v>407</v>
       </c>
@@ -4605,13 +5116,16 @@
         <v>317</v>
       </c>
       <c r="E142" s="6" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="F142" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G142" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A143" s="2" t="s">
         <v>407</v>
       </c>
@@ -4625,13 +5139,16 @@
         <v>319</v>
       </c>
       <c r="E143" s="6" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="F143" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G143" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
         <v>407</v>
       </c>
@@ -4645,13 +5162,16 @@
         <v>318</v>
       </c>
       <c r="E144" s="6" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="F144" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G144" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
         <v>407</v>
       </c>
@@ -4665,13 +5185,16 @@
         <v>320</v>
       </c>
       <c r="E145" s="6" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="F145" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G145" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
         <v>407</v>
       </c>
@@ -4685,13 +5208,16 @@
         <v>321</v>
       </c>
       <c r="E146" s="6" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="F146" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G146" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A147" s="2" t="s">
         <v>407</v>
       </c>
@@ -4705,13 +5231,16 @@
         <v>322</v>
       </c>
       <c r="E147" s="6" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="F147" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G147" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
         <v>407</v>
       </c>
@@ -4725,13 +5254,16 @@
         <v>323</v>
       </c>
       <c r="E148" s="6" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
       <c r="F148" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G148" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
         <v>407</v>
       </c>
@@ -4745,13 +5277,16 @@
         <v>324</v>
       </c>
       <c r="E149" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="F149" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="F149" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G149" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
         <v>407</v>
       </c>
@@ -4765,13 +5300,16 @@
         <v>325</v>
       </c>
       <c r="E150" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="F150" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="F150" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G150" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A151" s="2" t="s">
         <v>407</v>
       </c>
@@ -4785,13 +5323,16 @@
         <v>326</v>
       </c>
       <c r="E151" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="F151" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="F151" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G151" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
         <v>407</v>
       </c>
@@ -4805,13 +5346,16 @@
         <v>327</v>
       </c>
       <c r="E152" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="F152" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="F152" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="G152" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
         <v>407</v>
       </c>
@@ -4828,10 +5372,13 @@
         <v>15</v>
       </c>
       <c r="F153" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G153" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
         <v>407</v>
       </c>
@@ -4848,10 +5395,13 @@
         <v>15</v>
       </c>
       <c r="F154" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G154" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A155" s="2" t="s">
         <v>407</v>
       </c>
@@ -4868,10 +5418,13 @@
         <v>15</v>
       </c>
       <c r="F155" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G155" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
         <v>407</v>
       </c>
@@ -4888,10 +5441,13 @@
         <v>15</v>
       </c>
       <c r="F156" s="9" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+      <c r="G156" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
         <v>407</v>
       </c>
@@ -4908,10 +5464,13 @@
         <v>16</v>
       </c>
       <c r="F157" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G157" s="11" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
         <v>407</v>
       </c>
@@ -4928,10 +5487,13 @@
         <v>16</v>
       </c>
       <c r="F158" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G158" s="11" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A159" s="2" t="s">
         <v>407</v>
       </c>
@@ -4948,10 +5510,13 @@
         <v>16</v>
       </c>
       <c r="F159" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G159" s="11" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
         <v>407</v>
       </c>
@@ -4968,10 +5533,13 @@
         <v>16</v>
       </c>
       <c r="F160" s="9" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>422</v>
+      </c>
+      <c r="G160" s="11" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
         <v>408</v>
       </c>
@@ -4985,13 +5553,16 @@
         <v>336</v>
       </c>
       <c r="E161" s="7" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="F161" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G161" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
         <v>408</v>
       </c>
@@ -5005,13 +5576,16 @@
         <v>337</v>
       </c>
       <c r="E162" s="7" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="F162" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G162" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A163" s="2" t="s">
         <v>408</v>
       </c>
@@ -5025,13 +5599,16 @@
         <v>338</v>
       </c>
       <c r="E163" s="7" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="F163" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G163" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A164" s="2" t="s">
         <v>408</v>
       </c>
@@ -5045,13 +5622,16 @@
         <v>339</v>
       </c>
       <c r="E164" s="7" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="F164" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G164" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A165" s="2" t="s">
         <v>408</v>
       </c>
@@ -5065,13 +5645,16 @@
         <v>340</v>
       </c>
       <c r="E165" s="7" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="F165" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+      <c r="G165" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A166" s="2" t="s">
         <v>408</v>
       </c>
@@ -5085,13 +5668,16 @@
         <v>341</v>
       </c>
       <c r="E166" s="7" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="F166" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+      <c r="G166" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A167" s="2" t="s">
         <v>408</v>
       </c>
@@ -5105,13 +5691,16 @@
         <v>342</v>
       </c>
       <c r="E167" s="7" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="F167" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+      <c r="G167" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>408</v>
       </c>
@@ -5125,13 +5714,16 @@
         <v>343</v>
       </c>
       <c r="E168" s="7" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="F168" s="9" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>427</v>
+      </c>
+      <c r="G168" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A169" s="2" t="s">
         <v>408</v>
       </c>
@@ -5148,10 +5740,13 @@
         <v>18</v>
       </c>
       <c r="F169" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G169" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A170" s="2" t="s">
         <v>408</v>
       </c>
@@ -5168,10 +5763,13 @@
         <v>18</v>
       </c>
       <c r="F170" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G170" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A171" s="2" t="s">
         <v>408</v>
       </c>
@@ -5188,10 +5786,13 @@
         <v>18</v>
       </c>
       <c r="F171" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G171" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A172" s="2" t="s">
         <v>408</v>
       </c>
@@ -5208,10 +5809,13 @@
         <v>18</v>
       </c>
       <c r="F172" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G172" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A173" s="2" t="s">
         <v>408</v>
       </c>
@@ -5225,13 +5829,16 @@
         <v>348</v>
       </c>
       <c r="E173" s="7" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="F173" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G173" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>408</v>
       </c>
@@ -5245,13 +5852,16 @@
         <v>349</v>
       </c>
       <c r="E174" s="7" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="F174" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G174" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A175" s="2" t="s">
         <v>408</v>
       </c>
@@ -5265,13 +5875,16 @@
         <v>350</v>
       </c>
       <c r="E175" s="7" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="F175" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G175" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A176" s="2" t="s">
         <v>408</v>
       </c>
@@ -5285,13 +5898,16 @@
         <v>351</v>
       </c>
       <c r="E176" s="7" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="F176" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G176" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A177" s="2" t="s">
         <v>408</v>
       </c>
@@ -5305,13 +5921,16 @@
         <v>352</v>
       </c>
       <c r="E177" s="7" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="F177" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G177" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A178" s="2" t="s">
         <v>408</v>
       </c>
@@ -5325,13 +5944,16 @@
         <v>353</v>
       </c>
       <c r="E178" s="7" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="F178" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G178" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A179" s="2" t="s">
         <v>408</v>
       </c>
@@ -5345,13 +5967,16 @@
         <v>354</v>
       </c>
       <c r="E179" s="7" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="F179" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G179" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A180" s="2" t="s">
         <v>408</v>
       </c>
@@ -5365,13 +5990,16 @@
         <v>355</v>
       </c>
       <c r="E180" s="7" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="F180" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G180" s="11" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A181" s="2" t="s">
         <v>408</v>
       </c>
@@ -5385,13 +6013,16 @@
         <v>356</v>
       </c>
       <c r="E181" s="7" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="F181" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G181" s="11" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A182" s="2" t="s">
         <v>408</v>
       </c>
@@ -5405,13 +6036,16 @@
         <v>357</v>
       </c>
       <c r="E182" s="7" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="F182" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G182" s="11" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A183" s="2" t="s">
         <v>408</v>
       </c>
@@ -5425,13 +6059,16 @@
         <v>358</v>
       </c>
       <c r="E183" s="7" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="F183" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G183" s="11" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A184" s="2" t="s">
         <v>408</v>
       </c>
@@ -5445,13 +6082,16 @@
         <v>359</v>
       </c>
       <c r="E184" s="7" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="F184" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G184" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A185" s="2" t="s">
         <v>408</v>
       </c>
@@ -5465,13 +6105,16 @@
         <v>360</v>
       </c>
       <c r="E185" s="7" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="F185" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G185" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A186" s="2" t="s">
         <v>408</v>
       </c>
@@ -5485,13 +6128,16 @@
         <v>361</v>
       </c>
       <c r="E186" s="7" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="F186" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G186" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A187" s="2" t="s">
         <v>408</v>
       </c>
@@ -5505,13 +6151,16 @@
         <v>362</v>
       </c>
       <c r="E187" s="7" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="F187" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G187" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A188" s="2" t="s">
         <v>408</v>
       </c>
@@ -5525,13 +6174,16 @@
         <v>363</v>
       </c>
       <c r="E188" s="7" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="F188" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G188" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A189" s="2" t="s">
         <v>408</v>
       </c>
@@ -5545,13 +6197,16 @@
         <v>364</v>
       </c>
       <c r="E189" s="7" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="F189" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G189" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A190" s="2" t="s">
         <v>408</v>
       </c>
@@ -5565,13 +6220,16 @@
         <v>365</v>
       </c>
       <c r="E190" s="7" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="F190" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G190" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A191" s="2" t="s">
         <v>408</v>
       </c>
@@ -5585,13 +6243,16 @@
         <v>366</v>
       </c>
       <c r="E191" s="7" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="F191" s="9" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>419</v>
+      </c>
+      <c r="G191" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A192" s="2" t="s">
         <v>408</v>
       </c>
@@ -5608,10 +6269,13 @@
         <v>20</v>
       </c>
       <c r="F192" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G192" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A193" s="2" t="s">
         <v>408</v>
       </c>
@@ -5628,10 +6292,13 @@
         <v>20</v>
       </c>
       <c r="F193" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G193" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A194" s="2" t="s">
         <v>408</v>
       </c>
@@ -5648,10 +6315,13 @@
         <v>20</v>
       </c>
       <c r="F194" s="9" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>425</v>
+      </c>
+      <c r="G194" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A195" s="2" t="s">
         <v>408</v>
       </c>
@@ -5668,7 +6338,10 @@
         <v>20</v>
       </c>
       <c r="F195" s="9" t="s">
-        <v>442</v>
+        <v>425</v>
+      </c>
+      <c r="G195" s="11" t="s">
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>